<commit_message>
add function for get total product and write in the excel
</commit_message>
<xml_diff>
--- a/data/inventory.xlsx
+++ b/data/inventory.xlsx
@@ -3,20 +3,22 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="19095" yWindow="0" windowWidth="9810" windowHeight="15585" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="11535" yWindow="2985" windowWidth="15945" windowHeight="11295" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="INGRESO" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="RESUMEN" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="ENTRADAS" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="SALIDAS" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="8">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -32,16 +34,98 @@
       <u val="single"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="0"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="0"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="0"/>
+      <sz val="16"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="16"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.7999816888943144"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.5999938962981048"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -49,15 +133,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,147 +518,284 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:O3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="11" t="inlineStr">
+        <is>
+          <t>PRODUCTOS</t>
+        </is>
+      </c>
+      <c r="G1" s="11" t="inlineStr">
+        <is>
+          <t>ENTRADAS</t>
+        </is>
+      </c>
+      <c r="L1" s="11" t="inlineStr">
+        <is>
+          <t>SALIDAS</t>
+        </is>
+      </c>
+    </row>
+    <row r="2"/>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>CODIGO</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>PRODUCTO</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>ENTRADAS</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>SALIDAS</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>STOCK</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>CODIGO</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>PRODUCTO</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>FECHA</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>CANTIDAD</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>CODIGO</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>PRODUCTO</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>FECHA</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>CANTIDAD</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="G1:J2"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="L1:O2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18" defaultRowHeight="15"/>
   <cols>
-    <col width="23.7109375" customWidth="1" style="1" min="1" max="1"/>
-    <col width="21.5703125" bestFit="1" customWidth="1" style="3" min="2" max="2"/>
+    <col width="23.7109375" customWidth="1" style="14" min="1" max="1"/>
+    <col width="21.5703125" bestFit="1" customWidth="1" style="12" min="2" max="2"/>
+    <col width="5.7109375" customWidth="1" style="12" min="6" max="6"/>
+    <col width="19.85546875" customWidth="1" style="12" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>codigo</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>producto</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>categoria</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>cantidad</t>
-        </is>
+      <c r="A1" s="13" t="inlineStr">
+        <is>
+          <t>ENTRADAS</t>
+        </is>
+      </c>
+      <c r="G1" s="8" t="inlineStr">
+        <is>
+          <t>TOTAL PRODUCTOS</t>
+        </is>
+      </c>
+      <c r="H1" s="5" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="G2" s="8" t="inlineStr">
+        <is>
+          <t>TOTAL ENTRADAS</t>
+        </is>
+      </c>
+      <c r="H2" s="5" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>CODIGO</t>
+        </is>
+      </c>
+      <c r="B3" s="4" t="inlineStr">
+        <is>
+          <t>PRODUCTO</t>
+        </is>
+      </c>
+      <c r="C3" s="4" t="inlineStr">
+        <is>
+          <t>CATEGORIA</t>
+        </is>
+      </c>
+      <c r="D3" s="4" t="inlineStr">
+        <is>
+          <t>CANTIDAD</t>
+        </is>
+      </c>
+      <c r="E3" s="4" t="inlineStr">
+        <is>
+          <t>FECHA</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="14" t="inlineStr">
         <is>
           <t>7806500168102</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>papel elite</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>limpieza</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+    <row r="5">
+      <c r="A5" s="14" t="inlineStr">
         <is>
           <t>8888890334137</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>gomitas de melatonina</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>farmacias</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+    <row r="6">
+      <c r="A6" s="14" t="inlineStr">
         <is>
           <t>7802215514326</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>galleta donuts costa</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>comida</t>
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+    <row r="7">
+      <c r="A7" s="14" t="inlineStr">
         <is>
           <t>9786075281698</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>manga berserk tomo 1</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>libros</t>
         </is>
       </c>
-      <c r="D5" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
+      <c r="D7" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="14" t="inlineStr">
         <is>
           <t>9786075286709</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <t>manga berserk tomo 2</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>libros</t>
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+    <row r="9">
+      <c r="A9" s="14" t="inlineStr">
         <is>
           <t>9786075289335</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>manga berserk tomo 3</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>libros</t>
         </is>
       </c>
     </row>
-    <row r="8"/>
-    <row r="9"/>
     <row r="10"/>
     <row r="11">
       <c r="C11" s="2" t="n"/>
@@ -554,7 +808,206 @@
     <row r="17">
       <c r="C17" s="2" t="n"/>
     </row>
+    <row r="18"/>
+    <row r="19"/>
+    <row r="20"/>
+    <row r="21"/>
+    <row r="22"/>
+    <row r="23"/>
+    <row r="24">
+      <c r="D24" s="2" t="n"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="18" defaultRowHeight="15"/>
+  <cols>
+    <col width="23.7109375" customWidth="1" style="14" min="1" max="1"/>
+    <col width="21.5703125" bestFit="1" customWidth="1" style="12" min="2" max="2"/>
+    <col width="5.7109375" customWidth="1" style="12" min="6" max="6"/>
+    <col width="19.42578125" customWidth="1" style="12" min="7" max="7"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="15" t="inlineStr">
+        <is>
+          <t>SALIDAS</t>
+        </is>
+      </c>
+      <c r="G1" s="9" t="inlineStr">
+        <is>
+          <t>TOTAL PRODUCTOS</t>
+        </is>
+      </c>
+      <c r="H1" s="10" t="n"/>
+    </row>
+    <row r="2">
+      <c r="G2" s="9" t="inlineStr">
+        <is>
+          <t>TOTAL ENTRADAS</t>
+        </is>
+      </c>
+      <c r="H2" s="10" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="inlineStr">
+        <is>
+          <t>CODIGO</t>
+        </is>
+      </c>
+      <c r="B3" s="7" t="inlineStr">
+        <is>
+          <t>PRODUCTO</t>
+        </is>
+      </c>
+      <c r="C3" s="7" t="inlineStr">
+        <is>
+          <t>CATEGORIA</t>
+        </is>
+      </c>
+      <c r="D3" s="7" t="inlineStr">
+        <is>
+          <t>CANTIDAD</t>
+        </is>
+      </c>
+      <c r="E3" s="7" t="inlineStr">
+        <is>
+          <t>FECHA</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="14" t="inlineStr">
+        <is>
+          <t>7806500168102</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>papel elite</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>limpieza</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="14" t="inlineStr">
+        <is>
+          <t>8888890334137</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>gomitas de melatonina</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>farmacias</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="14" t="inlineStr">
+        <is>
+          <t>7802215514326</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>galleta donuts costa</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>comida</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="14" t="inlineStr">
+        <is>
+          <t>9786075281698</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>manga berserk tomo 1</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>libros</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="14" t="inlineStr">
+        <is>
+          <t>9786075286709</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>manga berserk tomo 2</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>libros</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="14" t="inlineStr">
+        <is>
+          <t>9786075289335</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>manga berserk tomo 3</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>libros</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" s="2" t="n"/>
+    </row>
+    <row r="17">
+      <c r="C17" s="2" t="n"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>